<commit_message>
tweaking colors and order
</commit_message>
<xml_diff>
--- a/PopGenome_Analysis/aesthetics/clock_scale.xlsx
+++ b/PopGenome_Analysis/aesthetics/clock_scale.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Seq/PopGenome_Analysis/aesthetics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2AF96DF-F2B3-564C-A49B-45645BD9F10C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDE6660-3529-084D-893D-AD4321048CFC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5580" yWindow="2360" windowWidth="27640" windowHeight="16940" xr2:uid="{8249347D-A98F-8F4E-A47E-543B58EB07CA}"/>
   </bookViews>
@@ -168,7 +168,7 @@
     <t>yscalar</t>
   </si>
   <si>
-    <t>xclockposition</t>
+    <t>yclockposition</t>
   </si>
 </sst>
 </file>
@@ -523,7 +523,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:H1048576"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>